<commit_message>
cleaning up my repro
</commit_message>
<xml_diff>
--- a/ARCHIVES/Master_RGB_Spreadsheet_AMMONIUM_Condensed_Red_5_3_23_need_to_be_fixed.xlsx
+++ b/ARCHIVES/Master_RGB_Spreadsheet_AMMONIUM_Condensed_Red_5_3_23_need_to_be_fixed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\Documents\PhD Boston University 2019-\Astrangia_nutrient_stressors_Rotjan_lab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\Documents\PhD Boston University 2019-\Chapter_2_Ecotox\Summer_2022_N_Ecotox\N_Ecotox_Chapter_2_ANALYSIS\Astrangia_nutrient_stressors_Rotjan_lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1F4751-E61D-476B-983C-308BA0E462ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFF703B-1B44-49E8-ABF9-23C7EEBEF920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="86280" yWindow="3525" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_data" sheetId="1" r:id="rId1"/>
@@ -9389,8 +9389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W479"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:U1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -48067,8 +48067,8 @@
   </sheetPr>
   <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J50" sqref="J50:J72"/>
     </sheetView>
   </sheetViews>

</xml_diff>